<commit_message>
bug OT .MA sur version anglaise
</commit_message>
<xml_diff>
--- a/templates/OT_.Ma.xlsx
+++ b/templates/OT_.Ma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gpm\www\GPM-TEST\lib\PHPExcel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F76453-99CC-4AF5-A41B-08E34C56B1FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F845EC-924C-4F6A-950D-2A965F4C3C48}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,9 +446,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,15 +485,27 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -511,15 +520,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -537,7 +537,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1371,8 +1406,8 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1391,85 +1426,85 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:11" ht="60.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G3" s="42"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="23"/>
-      <c r="G5" s="42"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="22"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="23"/>
-      <c r="G6" s="42"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="22"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="G7" s="42"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="G8" s="42"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="11" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
       <c r="F13" s="9" t="s">
         <v>6</v>
       </c>
@@ -1483,31 +1518,31 @@
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
@@ -1519,16 +1554,16 @@
       <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:13" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
     </row>
     <row r="21" spans="1:13" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
@@ -1536,39 +1571,39 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="24"/>
+      <c r="D21" s="23"/>
       <c r="F21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="30"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
     </row>
     <row r="22" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="24"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="25" t="s">
+      <c r="D23" s="25"/>
+      <c r="E23" s="24" t="s">
         <v>35</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
       <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1576,34 +1611,34 @@
         <v>15</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
     </row>
     <row r="26" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
       <c r="D26" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
     </row>
     <row r="27" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="31"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1611,26 +1646,26 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:H26"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:G8"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:H26"/>
   </mergeCells>
   <conditionalFormatting sqref="A23:D23">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$D23="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23 F23">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$F23="NO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1650,10 +1685,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+      <selection activeCell="C22" sqref="C22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1672,74 +1707,74 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:11" ht="60.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G3" s="42"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="19"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="17"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="18"/>
-      <c r="G6" s="42"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="17"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18"/>
-      <c r="G7" s="42"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18"/>
-      <c r="G8" s="42"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="11" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
       <c r="F13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1753,125 +1788,125 @@
       <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+    <row r="19" spans="1:13" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-    </row>
-    <row r="21" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+    </row>
+    <row r="21" spans="1:13" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25" t="s">
+      <c r="D21" s="23"/>
+      <c r="F21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
+    </row>
+    <row r="22" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="6"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-    </row>
-    <row r="26" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37" t="s">
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+    </row>
+    <row r="26" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
       <c r="D26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="43"/>
       <c r="B27" s="44"/>
       <c r="C27" s="45"/>
@@ -1883,6 +1918,7 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C22:H22"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="C2:F2"/>
@@ -1892,14 +1928,18 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A19:H19"/>
-    <mergeCell ref="C23:H23"/>
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="E26:H26"/>
   </mergeCells>
-  <conditionalFormatting sqref="E21:F22">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$F21="NO"</formula>
+  <conditionalFormatting sqref="A23:D23">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$D23="NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:F23">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$F23="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.35433070866141736" bottom="0.55118110236220474" header="0.11811023622047245" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
re-fix id ep 2E6 + recup OT .Ma
</commit_message>
<xml_diff>
--- a/templates/OT_.Ma.xlsx
+++ b/templates/OT_.Ma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gpm\www\GPM-TEST\lib\PHPExcel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GPM\www\GPM\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F76453-99CC-4AF5-A41B-08E34C56B1FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4CB8645-471F-4882-970B-0438797006EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSTT FR" sheetId="1" r:id="rId1"/>
@@ -446,9 +446,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,6 +485,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -537,7 +537,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1371,8 +1376,8 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1406,50 +1411,50 @@
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="22"/>
       <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="22"/>
       <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="G7" s="42"/>
     </row>
     <row r="8" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
       <c r="G8" s="42"/>
     </row>
     <row r="11" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1468,8 +1473,8 @@
       <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
       <c r="F13" s="9" t="s">
         <v>6</v>
       </c>
@@ -1483,9 +1488,9 @@
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
     </row>
@@ -1493,10 +1498,10 @@
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
     </row>
@@ -1505,7 +1510,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="F16" s="17"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
     </row>
@@ -1536,12 +1541,12 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="24"/>
+      <c r="D21" s="23"/>
       <c r="F21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="30"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
     </row>
     <row r="22" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
@@ -1560,15 +1565,15 @@
       <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="24"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="25" t="s">
+      <c r="D23" s="25"/>
+      <c r="E23" s="24" t="s">
         <v>35</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
       <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1603,7 +1608,7 @@
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="33"/>
-      <c r="D27" s="31"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1625,12 +1630,12 @@
     <mergeCell ref="E26:H26"/>
   </mergeCells>
   <conditionalFormatting sqref="A23:D23">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$D23="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23 F23">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$F23="NO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1650,10 +1655,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1687,39 +1692,39 @@
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="19"/>
       <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="17"/>
       <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="17"/>
       <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17"/>
       <c r="G7" s="42"/>
     </row>
     <row r="8" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
       <c r="G8" s="42"/>
     </row>
     <row r="11" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1738,8 +1743,8 @@
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
       <c r="F13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1753,9 +1758,9 @@
       <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
     </row>
@@ -1763,9 +1768,9 @@
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
     </row>
@@ -1773,24 +1778,24 @@
       <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-      <c r="F16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
         <v>11</v>
       </c>
@@ -1802,48 +1807,48 @@
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
     </row>
-    <row r="21" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25" t="s">
+      <c r="D21" s="23"/>
+      <c r="F21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
+    </row>
+    <row r="22" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="6"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
@@ -1855,7 +1860,7 @@
       <c r="G24" s="36"/>
       <c r="H24" s="36"/>
     </row>
-    <row r="26" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>30</v>
       </c>
@@ -1871,7 +1876,7 @@
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
     </row>
-    <row r="27" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="43"/>
       <c r="B27" s="44"/>
       <c r="C27" s="45"/>
@@ -1883,6 +1888,7 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C22:H22"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="C2:F2"/>
@@ -1892,14 +1898,18 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A19:H19"/>
-    <mergeCell ref="C23:H23"/>
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="E26:H26"/>
   </mergeCells>
-  <conditionalFormatting sqref="E21:F22">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$F21="NO"</formula>
+  <conditionalFormatting sqref="A23:D23">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$D23="NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:F23">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$F23="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.35433070866141736" bottom="0.55118110236220474" header="0.11811023622047245" footer="0.31496062992125984"/>

</xml_diff>